<commit_message>
XSSF Cell Formats, Sample Cells POC
</commit_message>
<xml_diff>
--- a/excel/CountryListProcessed.xlsx
+++ b/excel/CountryListProcessed.xlsx
@@ -20,7 +20,7 @@
     <t>India</t>
   </si>
   <si>
-    <t>can travel</t>
+    <t>quarantine</t>
   </si>
   <si>
     <t>AFG</t>
@@ -35,13 +35,13 @@
     <t>United States of America</t>
   </si>
   <si>
-    <t>restricted travel</t>
-  </si>
-  <si>
     <t>AIA</t>
   </si>
   <si>
     <t>Anguilla</t>
+  </si>
+  <si>
+    <t>can travel</t>
   </si>
 </sst>
 </file>
@@ -122,18 +122,18 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>